<commit_message>
Just comparing data sheets MAX30100 isn't useful here
</commit_message>
<xml_diff>
--- a/Mussel_heartrate_daughterboard/Mussel_heartrate_daughterboard_BOM_RevB.xlsx
+++ b/Mussel_heartrate_daughterboard/Mussel_heartrate_daughterboard_BOM_RevB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Hardware_projects\MusselHeartRate\Mussel_heartrate_daughterboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5296C8-19F3-412A-89EF-49FF821ADB27}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A047529D-5DC9-436C-87C4-EA54532F709A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="2140" windowWidth="18950" windowHeight="18310" xr2:uid="{4AA2F084-EC51-4134-827C-AE7E059FA00E}"/>
+    <workbookView xWindow="7020" yWindow="2450" windowWidth="30060" windowHeight="14480" xr2:uid="{4AA2F084-EC51-4134-827C-AE7E059FA00E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -677,7 +677,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="A1:F26"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>